<commit_message>
support specification date format
</commit_message>
<xml_diff>
--- a/tests/books/2/Book2.xlsx
+++ b/tests/books/2/Book2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryosuke/repositories/excel2json/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryosuke/repositories/excel2dict/tests/books/2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD6BD11-9FF4-2D43-9C0B-7A018F4849F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F37AAA-5400-2541-A88C-93814285A320}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="28300" windowHeight="16420" xr2:uid="{6F0C555D-B3A9-8C47-B1C8-48A845662D7D}"/>
   </bookViews>
@@ -517,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69980F66-1191-2F4C-9B08-0DEF6515AAA8}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -530,9 +530,10 @@
     <col min="5" max="5" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -555,7 +556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -577,8 +578,10 @@
       <c r="G2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="2"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -600,8 +603,10 @@
       <c r="G3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="2"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -623,38 +628,40 @@
       <c r="G4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="2"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="C5" s="1"/>
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9">
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:9">
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:9">
       <c r="C10" s="1"/>
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:9">
       <c r="C11" s="1"/>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>

</xml_diff>